<commit_message>
[add] beginning of analysis in r and some processors
</commit_message>
<xml_diff>
--- a/BOILERS/rkurs/FinalCodes.xlsx
+++ b/BOILERS/rkurs/FinalCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kocha\source\repos\itmo-viud\BOILERS\rkurs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C606D8-8CC5-4778-9166-7529FB5B0374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5F561F-E0F1-472B-B96A-FD0828AF290F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -3449,7 +3449,7 @@
   <dimension ref="A1:J972"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>